<commit_message>
Changed the name, ORCID end ROR codes.
</commit_message>
<xml_diff>
--- a/specimen_template.xlsx
+++ b/specimen_template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrooggioni/Sites/GitHub/specimen_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8F5CA345-BA3B-1F42-89C3-1B08DE2FD37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E7BD12-839C-0D47-9E99-A74A9F576257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecimentsInfo" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="219">
   <si>
     <t>term</t>
   </si>
@@ -399,15 +399,6 @@
     <t>https://deims.org/activity/50d7a52d-e384-4ed4-9976-5bf9c8302843</t>
   </si>
   <si>
-    <t>Andrea Lami</t>
-  </si>
-  <si>
-    <t>https://ror.org/02db0kh50</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0003-3627-0363</t>
-  </si>
-  <si>
     <t>Description of the sample</t>
   </si>
   <si>
@@ -621,15 +612,6 @@
     <t>sequential number</t>
   </si>
   <si>
-    <t>Alessandro Oggioni</t>
-  </si>
-  <si>
-    <t>https://ror.org/02wxw4x45</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0002-7997-219X</t>
-  </si>
-  <si>
     <t>name and surname</t>
   </si>
   <si>
@@ -657,12 +639,6 @@
     <t>use the number of specimen to which the curator's information refered</t>
   </si>
   <si>
-    <t>Michela Rogora</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0003-3515-0220</t>
-  </si>
-  <si>
     <t>resource Provider</t>
   </si>
   <si>
@@ -694,12 +670,39 @@
   </si>
   <si>
     <t>author</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-3327</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-3515</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-7997</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0003-3627</t>
+  </si>
+  <si>
+    <t>Mario Rossi</t>
+  </si>
+  <si>
+    <t>Jane Doe</t>
+  </si>
+  <si>
+    <t>Kovács János</t>
+  </si>
+  <si>
+    <t>https://ror.org/02db0k</t>
+  </si>
+  <si>
+    <t>https://ror.org/02wxw</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1684,7 +1687,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q100"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1694,14 +1697,14 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="13" width="18.1640625" customWidth="1"/>
-    <col min="14" max="14" width="18.1640625" hidden="1"/>
-    <col min="15" max="17" width="28.6640625" hidden="1"/>
+    <col min="14" max="14" width="18.1640625" hidden="1" customWidth="1"/>
+    <col min="15" max="17" width="28.6640625" hidden="1" customWidth="1"/>
     <col min="18" max="16384" width="18.1640625" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>97</v>
@@ -1710,7 +1713,7 @@
         <v>98</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>99</v>
@@ -1725,7 +1728,7 @@
         <v>102</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>110</v>
@@ -1737,15 +1740,15 @@
         <v>104</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>107</v>
@@ -1766,7 +1769,7 @@
         <v>109</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>110</v>
@@ -1778,7 +1781,7 @@
         <v>112</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -1792,7 +1795,7 @@
         <v>113</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>56</v>
@@ -1819,7 +1822,7 @@
         <v>118</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -1856,7 +1859,7 @@
         <v>118</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3302,10 +3305,10 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="5pesW2IcRb61HTCrN9rGxXs4fXJ9fN8ALIIHETOPoiE+9qJlXE46E+pUY6OvKwFhftmwBkDRrhQtqhJSPqq1fQ==" saltValue="yYnFT3UhDrvAdQlAV9T7Ag==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J102">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J102" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B102" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"true,false"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3313,25 +3316,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>resourceType!$A$2:$A$28</xm:f>
           </x14:formula1>
           <xm:sqref>E4:E102</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>mediumType!$A$2:$A$21</xm:f>
           </x14:formula1>
           <xm:sqref>F4:F102</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
             <xm:f>identifierType!$A$2:$A$15</xm:f>
           </x14:formula1>
           <xm:sqref>O101:O102</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000005000000}">
           <x14:formula1>
             <xm:f>relationType!$A$2:$A$5</xm:f>
           </x14:formula1>
@@ -3344,11 +3347,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -3363,16 +3366,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>105</v>
@@ -3380,19 +3383,19 @@
     </row>
     <row r="2" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>108</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -3400,16 +3403,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>119</v>
+        <v>216</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>121</v>
+        <v>210</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -3417,16 +3420,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3434,16 +3437,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -3451,16 +3454,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>119</v>
+        <v>216</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>121</v>
+        <v>213</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>120</v>
+        <v>217</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4122,12 +4125,12 @@
       <c r="E100" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Ff5UlYhFZYrTZVUjVAnoiPaAs9ZXNoKtF8pBRR4kuQam3HH8K5rcm988ypuHWpqKzR7Tfx1DYst0jQlC4hv2JA==" saltValue="r1bSB3LP5jgHucGOCalC+w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="boLedeO4g1swdtVku7qiRI+JVxPNBpgIBq0J78pVaHvRrTYWpxuuca1D4sP3Zg0WX4lM8PzvYlmz4oWSbgU+MA==" saltValue="ZeHgmmZzIWMOsOphWblphw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>conctactPersonType!$B$2:$B$12</xm:f>
           </x14:formula1>
@@ -4140,7 +4143,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
@@ -4158,30 +4161,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>106</v>
       </c>
       <c r="C1" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="D1" s="18" t="s">
         <v>179</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4189,13 +4192,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>111</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4203,13 +4206,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>111</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -4506,13 +4509,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>relationType!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>D3:D100</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>identifierType!$A$2:$A$15</xm:f>
           </x14:formula1>
@@ -4525,7 +4528,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4541,10 +4544,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -4552,123 +4555,123 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="C6" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B7" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B8" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="C8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B10" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B11" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="C11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="C12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -4678,7 +4681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5038,7 +5041,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5318,7 +5321,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5333,7 +5336,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>58</v>
@@ -5341,10 +5344,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5352,71 +5355,71 @@
         <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B11" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5424,15 +5427,15 @@
         <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -5440,15 +5443,15 @@
         <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -5458,7 +5461,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5473,7 +5476,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>58</v>
@@ -5481,34 +5484,34 @@
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new version of catalogue files
</commit_message>
<xml_diff>
--- a/specimen_template.xlsx
+++ b/specimen_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrooggioni/Sites/GitHub/specimen_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E7BD12-839C-0D47-9E99-A74A9F576257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E2C1C5-7906-8C43-96F9-37D23F0CFC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="45120" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecimentsInfo" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="218">
   <si>
     <t>term</t>
   </si>
@@ -390,9 +390,6 @@
     <t>https://deims.org/f30007c4-8a6e-4f11-ab87-569db54638fe</t>
   </si>
   <si>
-    <t>https://deims.org/locations/4930521a-596f-4e6f-90b8-29696b8c1c98</t>
-  </si>
-  <si>
     <t>https://doi.org/10.1007/BF02544119</t>
   </si>
   <si>
@@ -672,18 +669,6 @@
     <t>author</t>
   </si>
   <si>
-    <t>https://orcid.org/0000-0003-3327</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0003-3515</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0002-7997</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0003-3627</t>
-  </si>
-  <si>
     <t>Mario Rossi</t>
   </si>
   <si>
@@ -693,10 +678,22 @@
     <t>Kovács János</t>
   </si>
   <si>
-    <t>https://ror.org/02db0k</t>
-  </si>
-  <si>
-    <t>https://ror.org/02wxw</t>
+    <t>Niskin bottle</t>
+  </si>
+  <si>
+    <t>Gravity Corer</t>
+  </si>
+  <si>
+    <t>https://ror.org/02db0kh50</t>
+  </si>
+  <si>
+    <t>https://ror.org/02wxw4x45</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-7997-219X</t>
+  </si>
+  <si>
+    <t>https://deims.org/locations/ec1a58f7-1aee-4e3f-bec3-4eb1516ee905</t>
   </si>
 </sst>
 </file>
@@ -1690,8 +1687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1704,7 +1701,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>97</v>
@@ -1713,7 +1710,7 @@
         <v>98</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E1" s="11" t="s">
         <v>99</v>
@@ -1728,7 +1725,7 @@
         <v>102</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J1" s="11" t="s">
         <v>110</v>
@@ -1740,15 +1737,15 @@
         <v>104</v>
       </c>
       <c r="M1" s="12" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>107</v>
@@ -1769,7 +1766,7 @@
         <v>109</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>110</v>
@@ -1781,7 +1778,7 @@
         <v>112</v>
       </c>
       <c r="M2" s="15" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -1795,7 +1792,7 @@
         <v>113</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>56</v>
@@ -1810,19 +1807,19 @@
         <v>115</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="J3" s="23">
         <v>39490</v>
       </c>
       <c r="K3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="M3" s="6" t="s">
-        <v>178</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -1847,19 +1844,19 @@
         <v>115</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>116</v>
+        <v>217</v>
       </c>
       <c r="J4" s="23">
         <v>45334</v>
       </c>
       <c r="K4" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="L4" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="L4" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="M4" s="6" t="s">
-        <v>178</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3303,7 +3300,7 @@
       <c r="M100" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5pesW2IcRb61HTCrN9rGxXs4fXJ9fN8ALIIHETOPoiE+9qJlXE46E+pUY6OvKwFhftmwBkDRrhQtqhJSPqq1fQ==" saltValue="yYnFT3UhDrvAdQlAV9T7Ag==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zl+0gp8BUPw2eJ3n1E+If9sOyVlTwdu4DxRKvoVZ98TFIRTql+d4rkY2x9uGycI9ppcxxTTHk0lIXVK3j++N8Q==" saltValue="1Bgrfwk3SE8gMBkr+cHCqg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <dataValidations count="2">
     <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J102" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
@@ -3350,8 +3347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -3366,16 +3363,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>146</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>147</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>105</v>
@@ -3383,19 +3380,19 @@
     </row>
     <row r="2" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>108</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -3403,16 +3400,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>210</v>
-      </c>
       <c r="E3" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -3420,16 +3417,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -3437,16 +3434,16 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -3454,16 +3451,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>213</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -4125,7 +4122,7 @@
       <c r="E100" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="boLedeO4g1swdtVku7qiRI+JVxPNBpgIBq0J78pVaHvRrTYWpxuuca1D4sP3Zg0WX4lM8PzvYlmz4oWSbgU+MA==" saltValue="ZeHgmmZzIWMOsOphWblphw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="WTdQcZC4qMaW0XVcR49ptbqjLQZCu1RbdC4mcqOTDhxJJ6X+JLtZV3esHH2LvMMjZ5fcMt0Rq8GWiD3KVE9ePA==" saltValue="rpkO9pjESN2Qu5bS3Nxl5A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4161,30 +4158,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>106</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>194</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4192,13 +4189,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>111</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -4206,13 +4203,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>111</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
@@ -4544,10 +4541,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>120</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>121</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -4555,123 +4552,123 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
         <v>123</v>
-      </c>
-      <c r="B2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
         <v>125</v>
-      </c>
-      <c r="B3" t="s">
-        <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" t="s">
         <v>127</v>
-      </c>
-      <c r="B4" t="s">
-        <v>201</v>
-      </c>
-      <c r="C4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
         <v>129</v>
-      </c>
-      <c r="B5" t="s">
-        <v>202</v>
-      </c>
-      <c r="C5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C6" t="s">
         <v>131</v>
-      </c>
-      <c r="B6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" t="s">
         <v>133</v>
-      </c>
-      <c r="B7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C8" t="s">
         <v>135</v>
-      </c>
-      <c r="B8" t="s">
-        <v>205</v>
-      </c>
-      <c r="C8" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C9" t="s">
         <v>137</v>
-      </c>
-      <c r="B9" t="s">
-        <v>206</v>
-      </c>
-      <c r="C9" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" t="s">
         <v>139</v>
-      </c>
-      <c r="B10" t="s">
-        <v>207</v>
-      </c>
-      <c r="C10" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11" t="s">
+        <v>207</v>
+      </c>
+      <c r="C11" t="s">
         <v>141</v>
-      </c>
-      <c r="B11" t="s">
-        <v>208</v>
-      </c>
-      <c r="C11" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" t="s">
         <v>143</v>
-      </c>
-      <c r="B12" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" t="s">
-        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -5336,7 +5333,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>58</v>
@@ -5344,10 +5341,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -5355,71 +5352,71 @@
         <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -5427,15 +5424,15 @@
         <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -5443,15 +5440,15 @@
         <v>94</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -5476,7 +5473,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>58</v>
@@ -5484,34 +5481,34 @@
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
template with new info
</commit_message>
<xml_diff>
--- a/specimen_template.xlsx
+++ b/specimen_template.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrooggioni/Sites/GitHub/specimen_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E2C1C5-7906-8C43-96F9-37D23F0CFC81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40542793-51EA-C940-A419-92E890A3AAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="45120" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SpecimentsInfo" sheetId="3" r:id="rId1"/>
+    <sheet name="SpecimenInfo" sheetId="3" r:id="rId1"/>
     <sheet name="CuratorsInfo" sheetId="9" r:id="rId2"/>
     <sheet name="RelationInfo" sheetId="10" r:id="rId3"/>
-    <sheet name="conctactPersonType" sheetId="5" r:id="rId4"/>
-    <sheet name="resourceType" sheetId="1" r:id="rId5"/>
-    <sheet name="mediumType" sheetId="2" r:id="rId6"/>
-    <sheet name="identifierType" sheetId="6" r:id="rId7"/>
-    <sheet name="relationType" sheetId="7" r:id="rId8"/>
+    <sheet name="SamplersInfo" sheetId="11" r:id="rId4"/>
+    <sheet name="conctactPersonType" sheetId="5" r:id="rId5"/>
+    <sheet name="resourceType" sheetId="1" r:id="rId6"/>
+    <sheet name="mediumType" sheetId="2" r:id="rId7"/>
+    <sheet name="identifierType" sheetId="6" r:id="rId8"/>
+    <sheet name="relationType" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="224">
   <si>
     <t>term</t>
   </si>
@@ -694,6 +695,24 @@
   </si>
   <si>
     <t>https://deims.org/locations/ec1a58f7-1aee-4e3f-bec3-4eb1516ee905</t>
+  </si>
+  <si>
+    <t>https://deims.org/locations/711f996c-bc08-41a9-b9dc-24a5fa8de9f6</t>
+  </si>
+  <si>
+    <t>Sample LG98_03</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>sampler_name</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>sampler_test</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1284,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1326,10 +1345,16 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1389,9 +1414,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1429,7 +1454,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1535,7 +1560,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1677,18 +1702,39 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
+</file>
+
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{425F1E8E-8260-6A40-BB07-9FC9FD4EA5D9}">
+  <we:reference id="db18cc72-1a17-45df-b60e-7ffb655e8af5" version="1.0.0.4" store="EXCatalog" storeType="EXCatalog"/>
+  <we:alternateReferences>
+    <we:reference id="WA104381701" version="1.0.0.4" store="it-IT" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1730,13 +1776,13 @@
       <c r="J1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="M1" s="17" t="s">
         <v>176</v>
       </c>
     </row>
@@ -1771,92 +1817,90 @@
       <c r="J2" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="20" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="68" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
+      <c r="A3" s="24">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="b">
+      <c r="B3" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="26">
         <v>39490</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="25" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
+      <c r="A4" s="24">
         <v>2</v>
       </c>
-      <c r="B4" s="6" t="b">
+      <c r="B4" s="25" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5" t="s">
+      <c r="C4" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="25"/>
+      <c r="E4" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="G4" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="H4" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="J4" s="23">
+      <c r="I4" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="J4" s="26">
         <v>45334</v>
       </c>
-      <c r="K4" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>212</v>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -3300,30 +3344,48 @@
       <c r="M100" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="zl+0gp8BUPw2eJ3n1E+If9sOyVlTwdu4DxRKvoVZ98TFIRTql+d4rkY2x9uGycI9ppcxxTTHk0lIXVK3j++N8Q==" saltValue="1Bgrfwk3SE8gMBkr+cHCqg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <dataValidations count="2">
-    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J102" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="12">
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J101:J102" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B102" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B4 B101:B102" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"true,false"</formula1>
     </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please insert a sequential number from first to the last sample." promptTitle="This field is mandatory" prompt="Please, insert a sequential number from first to the last sample." sqref="A5:A100" xr:uid="{2B3F7CC3-B348-C846-AD01-0905C0768E07}">
+      <formula1>1</formula1>
+      <formula2>100</formula2>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please, provide a sample's title." promptTitle="This field is mandatory" prompt="Please, provide a sample's title." sqref="C5:C100" xr:uid="{D6CAC21E-405D-FA43-88D5-68B803119F22}">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="This field is optional" prompt="Please, add a valid activity's DEIMS.ID provided by the website deims.org." sqref="L5:L100" xr:uid="{AEE77905-4325-7746-8B83-3E294DD42A36}"/>
+    <dataValidation type="date" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please, insert the date when this sample has been collected with valid format (see the example above)." promptTitle="This field is mandatory" prompt="Please, insert the date when this sample has been collected with valid format (see the example above)." sqref="J5:J100" xr:uid="{808485A4-FAF2-B047-B833-6612B2A1C61E}">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please, select one of the option proposed. Select TRUE if the information of this sample will be public, otherwise select FALSE." promptTitle="This field is mandatory" prompt="Please, select one of the option proposed. Select TRUE if the information of this sample will be public, otherwise select FALSE." sqref="B5:B100" xr:uid="{BD2453C3-4887-D745-B0FF-9F7A97D68669}">
+      <formula1>"true,false"</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="This field is optional" prompt="Plesae, here provide the DOI of the method used to collect this sample." sqref="K5:K100" xr:uid="{8D5A9B56-3CA3-0446-9DC6-56401F8A2734}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="This field is optional" prompt="Please, insert here a simple text about why do you collect this sample." sqref="G5:G100" xr:uid="{7A35C9DB-C6F8-1A4D-B9BB-8D801144E02D}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please, add a valid site's DEIMS.ID provided by the website deims.org." promptTitle="This field is mandatory" prompt="Please, add a valid site's DEIMS.ID provided by the website deims.org." sqref="H5:H100" xr:uid="{04927102-3A0E-1D43-BE4C-35C3CD23E83A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please, add a valid location's DEIMS.ID provided by the website deims.org." promptTitle="This field is mandatory" prompt="Please, add a valid location's DEIMS.ID provided by the website deims.org." sqref="I5:I100" xr:uid="{53A18F92-C46F-7244-86D2-B160A4043545}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="This field is optional" prompt="Plesae, provide few words for describe this sample." sqref="D5:D100" xr:uid="{B457EFFB-E0BC-D648-AD97-E3FE7EC8D47E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000002000000}">
           <x14:formula1>
             <xm:f>resourceType!$A$2:$A$28</xm:f>
           </x14:formula1>
-          <xm:sqref>E4:E102</xm:sqref>
+          <xm:sqref>E4 E101:E102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>mediumType!$A$2:$A$21</xm:f>
           </x14:formula1>
-          <xm:sqref>F4:F102</xm:sqref>
+          <xm:sqref>F4 F101:F102</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000004000000}">
           <x14:formula1>
@@ -3337,6 +3399,30 @@
           </x14:formula1>
           <xm:sqref>P101:P102</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8A389CE4-46C1-D54E-B992-859FCB833816}">
+          <x14:formula1>
+            <xm:f>SamplersInfo!$A$3:$A$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>M3:M4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please, select one of the option proposed." promptTitle="This field is mandatory" prompt="Please, select one of the option proposed." xr:uid="{B158680E-8A15-7845-BEC9-BFC13ADBA60D}">
+          <x14:formula1>
+            <xm:f>resourceType!$A$2:$A$28</xm:f>
+          </x14:formula1>
+          <xm:sqref>E5:E100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please, select one of the option proposed." promptTitle="This field is mandatory" prompt="Please, select one of the option proposed." xr:uid="{473B8091-39A4-AF4F-AE4C-9C5170468923}">
+          <x14:formula1>
+            <xm:f>mediumType!$A$2:$A$21</xm:f>
+          </x14:formula1>
+          <xm:sqref>F5:F100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" promptTitle="This field is optional" prompt="Please, select one of the option proposed. If you want to add a new sampler please fill the table &quot;SamplersInfo&quot; in this file." xr:uid="{C5859399-2ABA-604E-9F5A-F1B1DA47FA02}">
+          <x14:formula1>
+            <xm:f>SamplersInfo!$A$3:$A$50</xm:f>
+          </x14:formula1>
+          <xm:sqref>M5:M100</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -3348,7 +3434,8 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView zoomScale="182" zoomScaleNormal="182" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4122,16 +4209,28 @@
       <c r="E100" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="WTdQcZC4qMaW0XVcR49ptbqjLQZCu1RbdC4mcqOTDhxJJ6X+JLtZV3esHH2LvMMjZ5fcMt0Rq8GWiD3KVE9ePA==" saltValue="rpkO9pjESN2Qu5bS3Nxl5A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="/QLj9K/1tyrf6I1pS2RNyAhdn3FPFyPHY8XNSoViBjldxFEIsraQ3w/Llq5MySfuOKf9bKJdLFPk8JceAZZE1Q==" saltValue="nJsUK3EoJs8FBEak+gjhTw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="4">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please provide a valid ROR ID (ror.org) for the institution to which the contact person belongs." promptTitle="This field is mandatory" prompt="Please provide a valid ROR ID (ror.org) for the institution to which the contact person belongs." sqref="E7:E100" xr:uid="{1591A8A3-9FF7-2945-B04C-CBF703B1F1D0}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please provide a valid ORCID for the person indicated in column B." promptTitle="This field is mandatory" prompt="Please provide a valid ORCID for the person indicated in column B." sqref="D7:D100" xr:uid="{17B2B21F-8036-D74B-8D55-555BA3F263CC}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please complete this cell with one of the sample numbers you used in the 'SpecimenInfo' table in this file. The information provided in this row refers to the sample associated with that number." promptTitle="This field is mandatory" prompt="Please complete this cell with one of the sample numbers you used in the 'SpecimenInfo' table in this file. The information provided in this row refers to the sample associated with that number." sqref="A7:A100" xr:uid="{0EA74AB3-65DF-B345-BBD1-CC26F95A7A92}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please provide the name of the contact person for the sample associated with the number provided in column A." promptTitle="This field is mandatory" prompt="Please provide the name of the contact person for the sample associated with the number provided in column A." sqref="B7:B100" xr:uid="{6096B1A2-BE79-FC41-85E3-0B8C5AE7F7A3}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>conctactPersonType!$B$2:$B$12</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C102</xm:sqref>
+          <xm:sqref>C3:C6 C101:C102</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="This field is mandatory" error="Please, select one of the proposed options to indicate the type of contact represented by the person in column B with respect to the sample." promptTitle="This field is mandatory" prompt="Please, select one of the proposed options to indicate the type of contact represented by the person in column B with respect to the sample." xr:uid="{20D6E198-C12F-734D-A5D4-B2CA26A047D5}">
+          <x14:formula1>
+            <xm:f>conctactPersonType!$B$2:$B$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>C7:C100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4144,7 +4243,8 @@
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView zoomScale="241" zoomScaleNormal="241" workbookViewId="0">
-      <selection sqref="A1:D4"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -4501,22 +4601,38 @@
       <c r="A100" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mB0TxkgKcsotO0GSEUZDMbCPyOSvNiBZ8AfjBOyVBIJtRnhkAQLjqu7k74kINlQU5WdiEPuspGnxc7oYJOZ5nQ==" saltValue="H5zccZJaJ8WEntQP1cYjVg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="q+5lbKkZ0RqR/L2WPvxR84GWv4R8gxVSBFFwsxN0pJRt14TnqVN2EL45YlNS12n/2KTFJzUPv+581Lscx2laxw==" saltValue="KrGUhLSTHhpPtahyNEDmag==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <dataValidations count="2">
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="This field is optional" prompt="Please complete this cell with one of the sample numbers you used in the 'SpecimenInfo' table in this file. The information provided in this row refers to the sample associated with that number." sqref="A5:A100" xr:uid="{A9E86395-EACB-D54F-9C9B-35E1CAE754C9}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" promptTitle="This field is optional" prompt="Indicate the PID (PID type is specified in column C) of the sample linked (relationship type is specified in column D) to the sample to which the number in column A refers." sqref="B5:B100" xr:uid="{921BB336-2481-504A-8C48-FF4F931FF7DC}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>relationType!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:D100</xm:sqref>
+          <xm:sqref>D3:D4</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>identifierType!$A$2:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>C3:C100</xm:sqref>
+          <xm:sqref>C3:C4</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select the type of PID provided in column B." xr:uid="{CBED5323-53CA-6A47-9E39-B15AB03D7630}">
+          <x14:formula1>
+            <xm:f>identifierType!$A$2:$A$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>C5:C100</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please select a relation type which combines the sample to which the number in column A refers and the sample to which the PID in column B refers." xr:uid="{3A9EC9AF-8499-B741-B54A-69A28FF0A176}">
+          <x14:formula1>
+            <xm:f>relationType!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5:D100</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4525,6 +4641,186 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10DA90EB-111B-904E-B004-7C938CD78E0F}">
+  <dimension ref="A1:A50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="10.83203125" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="8"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="8"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="8"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="8"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="8"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="8"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="8"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="8"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="8"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" s="8"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="8"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" s="8"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="8"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="8"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" s="8"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" s="8"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" s="8"/>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="8"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" s="8"/>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" s="8"/>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" s="8"/>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" s="8"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" s="8"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" s="8"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" s="8"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" s="8"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="8"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" s="8"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="8"/>
+    </row>
+  </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="x6mR0EiJ/2nO562Bglih8Cjw8BqXhGxq43+AS+uN958f2m7phosZAPpu7hIDgJIoIoDf1m0sXODPsEB8QXWq9g==" saltValue="o4g1pju+++2QcHOuzk0EQw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
@@ -4540,7 +4836,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>119</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -4677,7 +4973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -5037,7 +5333,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H21"/>
   <sheetViews>
@@ -5317,7 +5613,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -5457,7 +5753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>

</xml_diff>

<commit_message>
codelists for medium types and specimen types
</commit_message>
<xml_diff>
--- a/specimen_template.xlsx
+++ b/specimen_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrooggioni/Sites/GitHub/specimen_catalogue/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40542793-51EA-C940-A419-92E890A3AAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D10616-8E25-764E-B691-B9B0E6F18BFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SpecimenInfo" sheetId="3" r:id="rId1"/>
@@ -1732,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
+    <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
@@ -4977,8 +4977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5008,8 +5008,8 @@
         <v>3</v>
       </c>
       <c r="B2" t="str">
-        <f>"http://vocabulary.odm2.org/specimentype/"&amp;A2&amp;"/"</f>
-        <v>http://vocabulary.odm2.org/specimentype/automated/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A2&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/automated/</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -5020,8 +5020,8 @@
         <v>5</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B28" si="0">"http://vocabulary.odm2.org/specimentype/"&amp;A3&amp;"/"</f>
-        <v>http://vocabulary.odm2.org/specimentype/biota/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A3&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/biota/</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -5032,8 +5032,8 @@
         <v>7</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/core/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A4&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/core/</v>
       </c>
       <c r="C4" t="s">
         <v>8</v>
@@ -5044,8 +5044,8 @@
         <v>9</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/coreHalfRound/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A5&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/coreHalfRound/</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -5056,8 +5056,8 @@
         <v>11</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/corePiece/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A6&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/corePiece/</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -5068,8 +5068,8 @@
         <v>13</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/coreQuarterRound/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A7&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/coreQuarterRound/</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -5080,8 +5080,8 @@
         <v>15</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/coreSection/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A8&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/coreSection/</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
@@ -5092,8 +5092,8 @@
         <v>17</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/coreSectionHalf/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A9&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/coreSectionHalf/</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
@@ -5104,8 +5104,8 @@
         <v>19</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/coreSub-Piece/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A10&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/coreSub-Piece/</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -5116,8 +5116,8 @@
         <v>21</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/coreWholeRound/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A11&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/coreWholeRound/</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -5128,8 +5128,8 @@
         <v>23</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/cuttings/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A12&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/cuttings/</v>
       </c>
       <c r="C12" t="s">
         <v>24</v>
@@ -5140,8 +5140,8 @@
         <v>25</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/dredge/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A13&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/dredge/</v>
       </c>
       <c r="C13" t="s">
         <v>26</v>
@@ -5152,8 +5152,8 @@
         <v>27</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/foliageDigestion/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A14&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/foliageDigestion/</v>
       </c>
       <c r="C14" t="s">
         <v>28</v>
@@ -5164,8 +5164,8 @@
         <v>29</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/foliageLeaching/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A15&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/foliageLeaching/</v>
       </c>
       <c r="C15" t="s">
         <v>30</v>
@@ -5176,8 +5176,8 @@
         <v>31</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/forestFloorDigestion/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A16&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/forestFloorDigestion/</v>
       </c>
       <c r="C16" t="s">
         <v>32</v>
@@ -5188,8 +5188,8 @@
         <v>33</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/grab/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A17&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/grab/</v>
       </c>
       <c r="C17" t="s">
         <v>34</v>
@@ -5200,8 +5200,8 @@
         <v>35</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/individualSample/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A18&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/individualSample/</v>
       </c>
       <c r="C18" t="s">
         <v>36</v>
@@ -5212,8 +5212,8 @@
         <v>37</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/litterFallDigestion/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A19&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/litterFallDigestion/</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -5224,8 +5224,8 @@
         <v>39</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/orientedCore/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A20&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/orientedCore/</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
@@ -5236,8 +5236,8 @@
         <v>41</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/other/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A21&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/other/</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -5248,8 +5248,8 @@
         <v>44</v>
       </c>
       <c r="B22" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/petriDishDryDeposition/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A22&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/petriDishDryDeposition/</v>
       </c>
       <c r="C22" t="s">
         <v>45</v>
@@ -5260,8 +5260,8 @@
         <v>46</v>
       </c>
       <c r="B23" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/precipitationBulk/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A23&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/precipitationBulk/</v>
       </c>
       <c r="C23" t="s">
         <v>47</v>
@@ -5272,8 +5272,8 @@
         <v>48</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/rockPowder/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A24&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/rockPowder/</v>
       </c>
       <c r="C24" t="s">
         <v>49</v>
@@ -5284,8 +5284,8 @@
         <v>50</v>
       </c>
       <c r="B25" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/standardReferenceSpecimen/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A25&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/standardReferenceSpecimen/</v>
       </c>
       <c r="C25" t="s">
         <v>51</v>
@@ -5296,8 +5296,8 @@
         <v>52</v>
       </c>
       <c r="B26" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/terrestrialSection/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A26&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/terrestrialSection/</v>
       </c>
       <c r="C26" t="s">
         <v>53</v>
@@ -5308,8 +5308,8 @@
         <v>54</v>
       </c>
       <c r="B27" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/theSpecimenTypeIsUnknown/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A27&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/theSpecimenTypeIsUnknown/</v>
       </c>
       <c r="C27" t="s">
         <v>55</v>
@@ -5320,15 +5320,15 @@
         <v>56</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/specimentype/thinSection/</v>
+        <f>"https://rdfdata.lteritalia.it/specimentype/"&amp;A28&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/specimentype/thinSection/</v>
       </c>
       <c r="C28" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6Jdqzan4gqXSNnOXBN/mbACH5jr9bGTAl34wexkNDqtIYt0+9MeqrSJ0SFPxegtJ7HV4fhuPBkFWuVie77+iAA==" saltValue="QELSXzQdD3Z5PXJF/SDgRw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ELwEl8C7MnCpwW3XeiNMhOITHB+BtT7RlaIL3HAH57beATGtDdmSncb3z/Gjr6j+i7UFccSRv7FOeaq0H0mmHA==" saltValue="n/z5ljTd8sUJKPPDwbCeYA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -5338,7 +5338,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5369,8 +5369,8 @@
         <v>59</v>
       </c>
       <c r="B2" t="str">
-        <f>"http://vocabulary.odm2.org/medium/"&amp;A2&amp;"/"</f>
-        <v>http://vocabulary.odm2.org/medium/air/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A2&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/air/</v>
       </c>
       <c r="C2" t="s">
         <v>60</v>
@@ -5381,8 +5381,8 @@
         <v>61</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B21" si="0">"http://vocabulary.odm2.org/medium/"&amp;A3&amp;"/"</f>
-        <v>http://vocabulary.odm2.org/medium/equipment/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A3&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/equipment/</v>
       </c>
       <c r="C3" t="s">
         <v>62</v>
@@ -5393,8 +5393,8 @@
         <v>63</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/gas/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A4&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/gas/</v>
       </c>
       <c r="C4" t="s">
         <v>64</v>
@@ -5405,8 +5405,8 @@
         <v>65</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/habitat/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A5&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/habitat/</v>
       </c>
       <c r="C5" t="s">
         <v>66</v>
@@ -5419,8 +5419,8 @@
         <v>67</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/ice/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A6&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/ice/</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
@@ -5431,8 +5431,8 @@
         <v>69</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/liquidAqueous/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A7&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/liquidAqueous/</v>
       </c>
       <c r="C7" t="s">
         <v>70</v>
@@ -5443,8 +5443,8 @@
         <v>71</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/liquidOrganic/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A8&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/liquidOrganic/</v>
       </c>
       <c r="C8" t="s">
         <v>72</v>
@@ -5455,8 +5455,8 @@
         <v>73</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/mineral/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A9&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/mineral/</v>
       </c>
       <c r="C9" t="s">
         <v>74</v>
@@ -5467,8 +5467,8 @@
         <v>75</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/notApplicable/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A10&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/notApplicable/</v>
       </c>
       <c r="C10" t="s">
         <v>76</v>
@@ -5479,8 +5479,8 @@
         <v>77</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/organism/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A11&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/organism/</v>
       </c>
       <c r="C11" t="s">
         <v>78</v>
@@ -5491,8 +5491,8 @@
         <v>41</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/other/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A12&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/other/</v>
       </c>
       <c r="C12" t="s">
         <v>42</v>
@@ -5503,8 +5503,8 @@
         <v>79</v>
       </c>
       <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/particulate/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A13&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/particulate/</v>
       </c>
       <c r="C13" t="s">
         <v>80</v>
@@ -5515,8 +5515,8 @@
         <v>81</v>
       </c>
       <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/regolith/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A14&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/regolith/</v>
       </c>
       <c r="C14" t="s">
         <v>82</v>
@@ -5528,8 +5528,8 @@
         <v>83</v>
       </c>
       <c r="B15" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/rock/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A15&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/rock/</v>
       </c>
       <c r="C15" t="s">
         <v>84</v>
@@ -5540,8 +5540,8 @@
         <v>85</v>
       </c>
       <c r="B16" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/sediment/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A16&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/sediment/</v>
       </c>
       <c r="C16" t="s">
         <v>86</v>
@@ -5552,8 +5552,8 @@
         <v>87</v>
       </c>
       <c r="B17" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/snow/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A17&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/snow/</v>
       </c>
       <c r="C17" t="s">
         <v>88</v>
@@ -5564,8 +5564,8 @@
         <v>89</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/soil/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A18&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/soil/</v>
       </c>
       <c r="C18" t="s">
         <v>90</v>
@@ -5576,8 +5576,8 @@
         <v>91</v>
       </c>
       <c r="B19" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/tissue/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A19&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/tissue/</v>
       </c>
       <c r="C19" t="s">
         <v>92</v>
@@ -5588,8 +5588,8 @@
         <v>93</v>
       </c>
       <c r="B20" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/unknown/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A20&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/unknown/</v>
       </c>
       <c r="C20" t="s">
         <v>94</v>
@@ -5600,15 +5600,15 @@
         <v>95</v>
       </c>
       <c r="B21" t="str">
-        <f t="shared" si="0"/>
-        <v>http://vocabulary.odm2.org/medium/vegetation/</v>
+        <f>"https://rdfdata.lteritalia.it/mediumType/"&amp;A21&amp;"/"</f>
+        <v>https://rdfdata.lteritalia.it/mediumType/vegetation/</v>
       </c>
       <c r="C21" t="s">
         <v>96</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NWzFhPuNuXehN0/3UnIxo2mLsTcz/xi+2Yynaxtfb0p+Ur9wsQV0myPbA/jXwTkiIiLuLXEAdJfx3DDcRFOveQ==" saltValue="8NOVJm5aKEAXDe8u4oLXbw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2+6o7AibF8Jw3TjeIm5syV6JCddWovRY9r7AIp1G6Pa9cUvRRHE4oCrM7yndfNSzflNMNt8OefWk1VIu/q6hPg==" saltValue="Nsytjua/ar5wWsLfUk76Cw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>